<commit_message>
PPT Atualizado RoadMap Improve finalizado - Revisao Pendente
</commit_message>
<xml_diff>
--- a/1.Define/Custos Servidores/Relatório sobre custos_revisadaPedro.xlsx
+++ b/1.Define/Custos Servidores/Relatório sobre custos_revisadaPedro.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruhan\Documents\TCC\Define\Custos Servidores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\preto\OneDrive\Documentos\Puc_Lean2016\1.Define\Custos Servidores\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C96AE92-0F26-4276-87CC-1214A40C4FF8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Gerais" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,17 @@
     <sheet name="AnaliseCustosLíquido" sheetId="5" r:id="rId4"/>
     <sheet name="QUESTIONAMENTOS" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ruhan Pablo Acosta Sanabria</author>
   </authors>
   <commentList>
-    <comment ref="E18" authorId="0" shapeId="0">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,12 +58,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ruhan Pablo Acosta Sanabria</author>
   </authors>
   <commentList>
-    <comment ref="G19" authorId="0" shapeId="0">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -130,12 +131,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ruhan Pablo Acosta Sanabria</author>
   </authors>
   <commentList>
-    <comment ref="G19" authorId="0" shapeId="0">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -488,7 +489,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
@@ -859,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -989,6 +990,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,12 +1038,10 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1072,7 +1074,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2" descr="http://pad.tre-pr.gov.br/pad/temas/images/bullet_peq.png"/>
+        <xdr:cNvPr id="1026" name="Picture 2" descr="http://pad.tre-pr.gov.br/pad/temas/images/bullet_peq.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1112,7 +1120,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif"/>
+        <xdr:cNvPr id="1028" name="Picture 4" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1152,7 +1166,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1029" name="Picture 5" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1192,7 +1212,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6" descr="Primeira"/>
+        <xdr:cNvPr id="1030" name="Picture 6" descr="Primeira">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1232,7 +1258,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1031" name="Picture 7" descr="Anterior"/>
+        <xdr:cNvPr id="1031" name="Picture 7" descr="Anterior">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1272,7 +1304,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1032" name="Picture 8" descr="Próxima"/>
+        <xdr:cNvPr id="1032" name="Picture 8" descr="Próxima">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1312,7 +1350,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1033" name="Picture 9" descr="Última"/>
+        <xdr:cNvPr id="1033" name="Picture 9" descr="Última">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1352,7 +1396,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1034" name="Picture 10" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1034" name="Picture 10" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1392,7 +1442,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1035" name="Picture 11" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1035" name="Picture 11" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1432,7 +1488,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1036" name="Picture 12" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg"/>
+        <xdr:cNvPr id="1036" name="Picture 12" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1472,7 +1534,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1037" name="Picture 13" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg"/>
+        <xdr:cNvPr id="1037" name="Picture 13" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1512,7 +1580,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1039" name="Picture 15" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif"/>
+        <xdr:cNvPr id="1039" name="Picture 15" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1552,7 +1626,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1040" name="Picture 16" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1040" name="Picture 16" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1592,7 +1672,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1041" name="Picture 17" descr="Primeira"/>
+        <xdr:cNvPr id="1041" name="Picture 17" descr="Primeira">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1632,7 +1718,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1042" name="Picture 18" descr="Anterior"/>
+        <xdr:cNvPr id="1042" name="Picture 18" descr="Anterior">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1672,7 +1764,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1043" name="Picture 19" descr="Próxima"/>
+        <xdr:cNvPr id="1043" name="Picture 19" descr="Próxima">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1712,7 +1810,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1044" name="Picture 20" descr="Última"/>
+        <xdr:cNvPr id="1044" name="Picture 20" descr="Última">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1752,7 +1856,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1045" name="Picture 21" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1045" name="Picture 21" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1792,7 +1902,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1046" name="Picture 22" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="1046" name="Picture 22" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1834,6 +1950,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="1047" name="Picture 23" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -1876,6 +1997,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="1048" name="Picture 24" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -1918,6 +2044,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="1049" name="Picture 25" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -1953,7 +2084,13 @@
     <xdr:ext cx="57150" cy="57150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 2" descr="http://pad.tre-pr.gov.br/pad/temas/images/bullet_peq.png"/>
+        <xdr:cNvPr id="24" name="Picture 2" descr="http://pad.tre-pr.gov.br/pad/temas/images/bullet_peq.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1988,7 +2125,13 @@
     <xdr:ext cx="47625" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 4" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif"/>
+        <xdr:cNvPr id="25" name="Picture 4" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2023,7 +2166,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 5" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="26" name="Picture 5" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2058,7 +2207,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 6" descr="Primeira"/>
+        <xdr:cNvPr id="27" name="Picture 6" descr="Primeira">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2093,7 +2248,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 7" descr="Anterior"/>
+        <xdr:cNvPr id="28" name="Picture 7" descr="Anterior">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2128,7 +2289,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 8" descr="Próxima"/>
+        <xdr:cNvPr id="29" name="Picture 8" descr="Próxima">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2163,7 +2330,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 9" descr="Última"/>
+        <xdr:cNvPr id="30" name="Picture 9" descr="Última">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2198,7 +2371,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 10" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="31" name="Picture 10" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2233,7 +2412,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 11" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="32" name="Picture 11" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2268,7 +2453,13 @@
     <xdr:ext cx="180975" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 12" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg"/>
+        <xdr:cNvPr id="33" name="Picture 12" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2303,7 +2494,13 @@
     <xdr:ext cx="180975" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 13" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg"/>
+        <xdr:cNvPr id="34" name="Picture 13" descr="http://pad.tre-pr.gov.br/pad/temas/images/vermelho.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2338,7 +2535,13 @@
     <xdr:ext cx="47625" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 15" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif"/>
+        <xdr:cNvPr id="35" name="Picture 15" descr="http://pad.tre-pr.gov.br/pad/temas/images/filterstart.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2373,7 +2576,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 16" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="36" name="Picture 16" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2408,7 +2617,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 17" descr="Primeira"/>
+        <xdr:cNvPr id="37" name="Picture 17" descr="Primeira">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2443,7 +2658,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 18" descr="Anterior"/>
+        <xdr:cNvPr id="38" name="Picture 18" descr="Anterior">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2478,7 +2699,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 19" descr="Próxima"/>
+        <xdr:cNvPr id="39" name="Picture 19" descr="Próxima">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2513,7 +2740,13 @@
     <xdr:ext cx="228600" cy="171450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 20" descr="Última"/>
+        <xdr:cNvPr id="40" name="Picture 20" descr="Última">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2548,7 +2781,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 21" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="41" name="Picture 21" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2583,7 +2822,13 @@
     <xdr:ext cx="76200" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 22" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif"/>
+        <xdr:cNvPr id="42" name="Picture 22" descr="http://pad.tre-pr.gov.br/pad/temas/images/separator.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2620,6 +2865,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="43" name="Picture 23" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2657,6 +2907,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="44" name="Picture 24" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2694,6 +2949,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="45" name="Picture 25" descr="http://pad.tre-pr.gov.br/pad/temas/images/tramitacao_processo/tramitacao_detalhe.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2723,9 +2983,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2763,7 +3023,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2798,6 +3058,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2833,9 +3110,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3008,10 +3302,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3027,12 +3321,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3115,12 +3409,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
       <c r="E9" t="s">
         <v>76</v>
       </c>
@@ -3188,7 +3482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -3206,27 +3500,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="69"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3290,7 +3584,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="70" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="39" t="s">
@@ -3314,7 +3608,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="39" t="s">
         <v>55</v>
       </c>
@@ -3336,7 +3630,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="39" t="s">
         <v>56</v>
       </c>
@@ -3358,7 +3652,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="39" t="s">
         <v>57</v>
       </c>
@@ -3380,7 +3674,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="39" t="s">
         <v>58</v>
       </c>
@@ -3402,8 +3696,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
-      <c r="B15" s="70" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="71" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="40">
@@ -3424,8 +3718,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -3579,7 +3873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -3611,22 +3905,22 @@
       <c r="C2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="75"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" s="78" t="s">
+      <c r="H3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="79"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="75"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -3637,10 +3931,10 @@
         <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="79">
+      <c r="H5" s="80">
         <v>0.15</v>
       </c>
-      <c r="I5" s="78"/>
+      <c r="I5" s="79"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -3658,10 +3952,10 @@
       <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="75"/>
+      <c r="I6" s="76"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3679,10 +3973,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="78"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -3700,10 +3994,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -3721,18 +4015,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="78"/>
+      <c r="I9" s="79"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -3741,36 +4035,36 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -3804,7 +4098,7 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="78" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3822,7 +4116,7 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -3838,7 +4132,7 @@
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="45" t="s">
         <v>1</v>
       </c>
@@ -3936,12 +4230,12 @@
       <c r="A22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
@@ -3968,14 +4262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:I22"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3989,6 +4283,7 @@
     <col min="7" max="7" width="42.28515625" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4000,26 +4295,26 @@
       <c r="C2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="75"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="78" t="s">
+      <c r="H3" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="78"/>
+      <c r="I3" s="79"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="75"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -4030,10 +4325,10 @@
         <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="79">
+      <c r="H5" s="80">
         <v>0.15</v>
       </c>
-      <c r="I5" s="78"/>
+      <c r="I5" s="79"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -4051,10 +4346,10 @@
       <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="75"/>
+      <c r="I6" s="76"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -4072,10 +4367,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="78"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4093,10 +4388,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4114,18 +4409,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="78"/>
+      <c r="I9" s="79"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -4134,38 +4429,38 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="76"/>
-    </row>
-    <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+    </row>
+    <row r="14" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="22" t="s">
         <v>12</v>
@@ -4195,13 +4490,13 @@
         <f>D15/30</f>
         <v>341.46623466666665</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="65" t="s">
         <v>72</v>
       </c>
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="78" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -4218,8 +4513,8 @@
       </c>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="78"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -4234,8 +4529,8 @@
       </c>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="1:9" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
+    <row r="18" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="78"/>
       <c r="B18" s="45" t="s">
         <v>1</v>
       </c>
@@ -4261,7 +4556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>17</v>
       </c>
@@ -4294,7 +4589,7 @@
         <v>1694905.2700799999</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>49</v>
       </c>
@@ -4317,8 +4612,15 @@
         <f>(3*(1320))*E19</f>
         <v>1694905.2700799999</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="J20" s="81">
+        <v>0.3</v>
+      </c>
+      <c r="K20" s="8">
+        <f>I20*J20</f>
+        <v>508471.58102399996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -4335,18 +4637,18 @@
         <v>1569.3567315555554</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
     </row>
   </sheetData>
@@ -4371,7 +4673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>

</xml_diff>